<commit_message>
Now does proper file dump on 'P'
</commit_message>
<xml_diff>
--- a/Simulation/Simulation/PIDChart.xlsx
+++ b/Simulation/Simulation/PIDChart.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="output" localSheetId="0">Sheet1!$A$1:$B$102</definedName>
+    <definedName name="output" localSheetId="0">Sheet1!$A$1:$C$63</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -156,630 +156,366 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$102</c:f>
+              <c:f>Sheet1!$A$1:$A$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="63"/>
                 <c:pt idx="0">
-                  <c:v>479031</c:v>
+                  <c:v>250100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>488804</c:v>
+                  <c:v>450200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>508356</c:v>
+                  <c:v>650300000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>527908</c:v>
+                  <c:v>850400000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>557236</c:v>
+                  <c:v>1450500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>625669</c:v>
+                  <c:v>1650600000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>763025</c:v>
+                  <c:v>1850700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1025455</c:v>
+                  <c:v>2450800000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1651136</c:v>
+                  <c:v>2650900000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2714582</c:v>
+                  <c:v>3251000000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19085976</c:v>
+                  <c:v>3451100000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27316713</c:v>
+                  <c:v>4051200000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30947211</c:v>
+                  <c:v>4251300000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32763229</c:v>
+                  <c:v>4851400000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>33676119</c:v>
+                  <c:v>6651500000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34135591</c:v>
+                  <c:v>12051600000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34587686</c:v>
+                  <c:v>12251700000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35508332</c:v>
+                  <c:v>12851800000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35958644</c:v>
+                  <c:v>14651900000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36864277</c:v>
+                  <c:v>20052000000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>53375782</c:v>
+                  <c:v>36252100000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>61837068</c:v>
+                  <c:v>36452200000</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>66061359</c:v>
+                  <c:v>37052300000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>68176197</c:v>
+                  <c:v>38852400000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>69236980</c:v>
+                  <c:v>44252500000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>69764884</c:v>
+                  <c:v>60452600000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>70296516</c:v>
+                  <c:v>60652700000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>71356042</c:v>
+                  <c:v>61252800000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>71896041</c:v>
+                  <c:v>63052900000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>72956963</c:v>
+                  <c:v>68453000000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>89908962</c:v>
+                  <c:v>84653100000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>98374854</c:v>
+                  <c:v>84853200000</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>102623009</c:v>
+                  <c:v>85453300000</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>104767801</c:v>
+                  <c:v>87253400000</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>105819864</c:v>
+                  <c:v>92653500000</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>106347438</c:v>
+                  <c:v>108853600000</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>106889821</c:v>
+                  <c:v>109053700000</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>107937140</c:v>
+                  <c:v>109653800000</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>108472270</c:v>
+                  <c:v>111453900000</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>109533182</c:v>
+                  <c:v>116854000000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>126575667</c:v>
+                  <c:v>133054100000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>135088820</c:v>
+                  <c:v>133254200000</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>139357285</c:v>
+                  <c:v>133854300000</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>139357285</c:v>
+                  <c:v>135654400000</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>140426597</c:v>
+                  <c:v>141054500000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>140967058</c:v>
+                  <c:v>157254600000</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>141231009</c:v>
+                  <c:v>157454700000</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>141367877</c:v>
+                  <c:v>158054800000</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>141436310</c:v>
+                  <c:v>159854900000</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>141475414</c:v>
+                  <c:v>165255000000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>141494969</c:v>
+                  <c:v>181455100000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>141524294</c:v>
+                  <c:v>181655200000</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>141593663</c:v>
+                  <c:v>182255300000</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>141723536</c:v>
+                  <c:v>184055400000</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>141987490</c:v>
+                  <c:v>189455500000</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>142525174</c:v>
+                  <c:v>205655600000</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>143605446</c:v>
+                  <c:v>205855700000</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>144676368</c:v>
+                  <c:v>206455800000</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>161841702</c:v>
+                  <c:v>208255900000</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>170508605</c:v>
+                  <c:v>213656000000</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>174842161</c:v>
+                  <c:v>229856100000</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>177033678</c:v>
+                  <c:v>278456200000</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>178099828</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>178636319</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>179176325</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>180245640</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>180787041</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>181846581</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>200870363</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>211532777</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>215825156</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>215834935</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>216913206</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>217453257</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>217723462</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>217848331</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>217926543</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>217965644</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>217985200</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>218019316</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>218084372</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>218213552</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>218500769</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>219124221</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>220193533</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>237354053</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>237359060</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>241587749</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>243729247</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>244784993</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>245315354</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>245585542</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>245720635</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>245785680</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>245820711</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>245840719</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>245875743</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>245940788</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>246075882</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>246341065</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>246871433</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>247932168</c:v>
+                  <c:v>424256300000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$102</c:f>
+              <c:f>Sheet1!$B$11:$B$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
-                  <c:v>1681</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1731</c:v>
+                  <c:v>3.33277787035494E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1881</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1929</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2017</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2053</c:v>
+                  <c:v>-3.7036351178681799E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2053</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2053</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2052</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2050</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2030</c:v>
+                  <c:v>-2.4691205609841901E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2122</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1933</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2080</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2060</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2057</c:v>
+                  <c:v>-2.4691205609841901E-5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2055</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2051</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2051</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2050</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2030</c:v>
+                  <c:v>-2.4691205609841901E-5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2122</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1933</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2080</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2060</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2057</c:v>
+                  <c:v>-1.23456028049209E-5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2055</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2051</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2051</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2050</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2030</c:v>
+                  <c:v>-1.23456028049209E-5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2122</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1933</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2080</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2060</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2057</c:v>
+                  <c:v>-1.23456028049209E-5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2055</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2051</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2051</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2050</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2030</c:v>
+                  <c:v>-1.23456028049209E-5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2122</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1933</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2227</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2113</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1733</c:v>
+                  <c:v>-1.23456028049209E-5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3533</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2533</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1621</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2021</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2021</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2021</c:v>
+                  <c:v>-8.2304357398441507E-6</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2057</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2057</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2056</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2054</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>2051</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>2050</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>2030</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2122</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1933</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2080</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2060</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>2057</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>2055</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>2051</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>2051</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>2050</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>2030</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>2122</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1933</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>2227</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>2113</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1733</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>3533</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>2533</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>1525</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>2044</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>2044</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>2045</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>2046</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>2066</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>1882</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>2307</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>1976</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>2174</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>1454</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>3522</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>690</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>2041</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>2043</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>2046</c:v>
+                  <c:v>-5.4869646865811402E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,318 +561,201 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$1:$B$102</c15:sqref>
+                          <c15:sqref>Sheet1!$A$1:$A$63</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="102"/>
+                      <c:ptCount val="63"/>
                       <c:pt idx="0">
-                        <c:v>479031</c:v>
+                        <c:v>250100000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>488804</c:v>
+                        <c:v>450200000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>508356</c:v>
+                        <c:v>650300000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>527908</c:v>
+                        <c:v>850400000</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>557236</c:v>
+                        <c:v>1450500000</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>625669</c:v>
+                        <c:v>1650600000</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>763025</c:v>
+                        <c:v>1850700000</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1025455</c:v>
+                        <c:v>2450800000</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>1651136</c:v>
+                        <c:v>2650900000</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>2714582</c:v>
+                        <c:v>3251000000</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>19085976</c:v>
+                        <c:v>3451100000</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>27316713</c:v>
+                        <c:v>4051200000</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>30947211</c:v>
+                        <c:v>4251300000</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>32763229</c:v>
+                        <c:v>4851400000</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>33676119</c:v>
+                        <c:v>6651500000</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>34135591</c:v>
+                        <c:v>12051600000</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>34587686</c:v>
+                        <c:v>12251700000</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>35508332</c:v>
+                        <c:v>12851800000</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>35958644</c:v>
+                        <c:v>14651900000</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>36864277</c:v>
+                        <c:v>20052000000</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>53375782</c:v>
+                        <c:v>36252100000</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>61837068</c:v>
+                        <c:v>36452200000</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>66061359</c:v>
+                        <c:v>37052300000</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>68176197</c:v>
+                        <c:v>38852400000</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>69236980</c:v>
+                        <c:v>44252500000</c:v>
                       </c:pt>
                       <c:pt idx="25">
-                        <c:v>69764884</c:v>
+                        <c:v>60452600000</c:v>
                       </c:pt>
                       <c:pt idx="26">
-                        <c:v>70296516</c:v>
+                        <c:v>60652700000</c:v>
                       </c:pt>
                       <c:pt idx="27">
-                        <c:v>71356042</c:v>
+                        <c:v>61252800000</c:v>
                       </c:pt>
                       <c:pt idx="28">
-                        <c:v>71896041</c:v>
+                        <c:v>63052900000</c:v>
                       </c:pt>
                       <c:pt idx="29">
-                        <c:v>72956963</c:v>
+                        <c:v>68453000000</c:v>
                       </c:pt>
                       <c:pt idx="30">
-                        <c:v>89908962</c:v>
+                        <c:v>84653100000</c:v>
                       </c:pt>
                       <c:pt idx="31">
-                        <c:v>98374854</c:v>
+                        <c:v>84853200000</c:v>
                       </c:pt>
                       <c:pt idx="32">
-                        <c:v>102623009</c:v>
+                        <c:v>85453300000</c:v>
                       </c:pt>
                       <c:pt idx="33">
-                        <c:v>104767801</c:v>
+                        <c:v>87253400000</c:v>
                       </c:pt>
                       <c:pt idx="34">
-                        <c:v>105819864</c:v>
+                        <c:v>92653500000</c:v>
                       </c:pt>
                       <c:pt idx="35">
-                        <c:v>106347438</c:v>
+                        <c:v>108853600000</c:v>
                       </c:pt>
                       <c:pt idx="36">
-                        <c:v>106889821</c:v>
+                        <c:v>109053700000</c:v>
                       </c:pt>
                       <c:pt idx="37">
-                        <c:v>107937140</c:v>
+                        <c:v>109653800000</c:v>
                       </c:pt>
                       <c:pt idx="38">
-                        <c:v>108472270</c:v>
+                        <c:v>111453900000</c:v>
                       </c:pt>
                       <c:pt idx="39">
-                        <c:v>109533182</c:v>
+                        <c:v>116854000000</c:v>
                       </c:pt>
                       <c:pt idx="40">
-                        <c:v>126575667</c:v>
+                        <c:v>133054100000</c:v>
                       </c:pt>
                       <c:pt idx="41">
-                        <c:v>135088820</c:v>
+                        <c:v>133254200000</c:v>
                       </c:pt>
                       <c:pt idx="42">
-                        <c:v>139357285</c:v>
+                        <c:v>133854300000</c:v>
                       </c:pt>
                       <c:pt idx="43">
-                        <c:v>139357285</c:v>
+                        <c:v>135654400000</c:v>
                       </c:pt>
                       <c:pt idx="44">
-                        <c:v>140426597</c:v>
+                        <c:v>141054500000</c:v>
                       </c:pt>
                       <c:pt idx="45">
-                        <c:v>140967058</c:v>
+                        <c:v>157254600000</c:v>
                       </c:pt>
                       <c:pt idx="46">
-                        <c:v>141231009</c:v>
+                        <c:v>157454700000</c:v>
                       </c:pt>
                       <c:pt idx="47">
-                        <c:v>141367877</c:v>
+                        <c:v>158054800000</c:v>
                       </c:pt>
                       <c:pt idx="48">
-                        <c:v>141436310</c:v>
+                        <c:v>159854900000</c:v>
                       </c:pt>
                       <c:pt idx="49">
-                        <c:v>141475414</c:v>
+                        <c:v>165255000000</c:v>
                       </c:pt>
                       <c:pt idx="50">
-                        <c:v>141494969</c:v>
+                        <c:v>181455100000</c:v>
                       </c:pt>
                       <c:pt idx="51">
-                        <c:v>141524294</c:v>
+                        <c:v>181655200000</c:v>
                       </c:pt>
                       <c:pt idx="52">
-                        <c:v>141593663</c:v>
+                        <c:v>182255300000</c:v>
                       </c:pt>
                       <c:pt idx="53">
-                        <c:v>141723536</c:v>
+                        <c:v>184055400000</c:v>
                       </c:pt>
                       <c:pt idx="54">
-                        <c:v>141987490</c:v>
+                        <c:v>189455500000</c:v>
                       </c:pt>
                       <c:pt idx="55">
-                        <c:v>142525174</c:v>
+                        <c:v>205655600000</c:v>
                       </c:pt>
                       <c:pt idx="56">
-                        <c:v>143605446</c:v>
+                        <c:v>205855700000</c:v>
                       </c:pt>
                       <c:pt idx="57">
-                        <c:v>144676368</c:v>
+                        <c:v>206455800000</c:v>
                       </c:pt>
                       <c:pt idx="58">
-                        <c:v>161841702</c:v>
+                        <c:v>208255900000</c:v>
                       </c:pt>
                       <c:pt idx="59">
-                        <c:v>170508605</c:v>
+                        <c:v>213656000000</c:v>
                       </c:pt>
                       <c:pt idx="60">
-                        <c:v>174842161</c:v>
+                        <c:v>229856100000</c:v>
                       </c:pt>
                       <c:pt idx="61">
-                        <c:v>177033678</c:v>
+                        <c:v>278456200000</c:v>
                       </c:pt>
                       <c:pt idx="62">
-                        <c:v>178099828</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>178636319</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>179176325</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>180245640</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>180787041</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>181846581</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>200870363</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>211532777</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>215825156</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>215834935</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>216913206</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>217453257</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>217723462</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>217848331</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>217926543</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>217965644</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>217985200</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>218019316</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>218084372</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>218213552</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>218500769</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>219124221</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>220193533</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>237354053</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>237359060</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>241587749</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>243729247</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>244784993</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>245315354</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>245585542</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>245720635</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>245785680</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>245820711</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>245840719</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>245875743</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>245940788</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>246075882</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>246341065</c:v>
-                      </c:pt>
-                      <c:pt idx="100">
-                        <c:v>246871433</c:v>
-                      </c:pt>
-                      <c:pt idx="101">
-                        <c:v>247932168</c:v>
+                        <c:v>424256300000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1146,318 +765,201 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$1:$B$102</c15:sqref>
+                          <c15:sqref>Sheet1!$B$1:$B$63</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="102"/>
+                      <c:ptCount val="63"/>
                       <c:pt idx="0">
-                        <c:v>479031</c:v>
+                        <c:v>9.5961615353858404E-3</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>488804</c:v>
+                        <c:v>-2.9985007496251799E-3</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>508356</c:v>
+                        <c:v>1.9990004997501201E-3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>527908</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>557236</c:v>
+                        <c:v>6.66555574070988E-4</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>625669</c:v>
+                        <c:v>9.99500249875062E-4</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>763025</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1025455</c:v>
+                        <c:v>3.33277787035494E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>1651136</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>2714582</c:v>
+                        <c:v>3.33277787035494E-4</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>19085976</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>27316713</c:v>
+                        <c:v>3.33277787035494E-4</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>30947211</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>32763229</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>33676119</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>34135591</c:v>
+                        <c:v>-3.7036351178681799E-5</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>34587686</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>35508332</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>35958644</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>36864277</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>53375782</c:v>
+                        <c:v>-2.4691205609841901E-5</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>61837068</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>66061359</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>68176197</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>69236980</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="25">
-                        <c:v>69764884</c:v>
+                        <c:v>-2.4691205609841901E-5</c:v>
                       </c:pt>
                       <c:pt idx="26">
-                        <c:v>70296516</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="27">
-                        <c:v>71356042</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="28">
-                        <c:v>71896041</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="29">
-                        <c:v>72956963</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="30">
-                        <c:v>89908962</c:v>
+                        <c:v>-2.4691205609841901E-5</c:v>
                       </c:pt>
                       <c:pt idx="31">
-                        <c:v>98374854</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="32">
-                        <c:v>102623009</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="33">
-                        <c:v>104767801</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="34">
-                        <c:v>105819864</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="35">
-                        <c:v>106347438</c:v>
+                        <c:v>-1.23456028049209E-5</c:v>
                       </c:pt>
                       <c:pt idx="36">
-                        <c:v>106889821</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="37">
-                        <c:v>107937140</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="38">
-                        <c:v>108472270</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="39">
-                        <c:v>109533182</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="40">
-                        <c:v>126575667</c:v>
+                        <c:v>-1.23456028049209E-5</c:v>
                       </c:pt>
                       <c:pt idx="41">
-                        <c:v>135088820</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="42">
-                        <c:v>139357285</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="43">
-                        <c:v>139357285</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="44">
-                        <c:v>140426597</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="45">
-                        <c:v>140967058</c:v>
+                        <c:v>-1.23456028049209E-5</c:v>
                       </c:pt>
                       <c:pt idx="46">
-                        <c:v>141231009</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="47">
-                        <c:v>141367877</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="48">
-                        <c:v>141436310</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="49">
-                        <c:v>141475414</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="50">
-                        <c:v>141494969</c:v>
+                        <c:v>-1.23456028049209E-5</c:v>
                       </c:pt>
                       <c:pt idx="51">
-                        <c:v>141524294</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="52">
-                        <c:v>141593663</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="53">
-                        <c:v>141723536</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="54">
-                        <c:v>141987490</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="55">
-                        <c:v>142525174</c:v>
+                        <c:v>-1.23456028049209E-5</c:v>
                       </c:pt>
                       <c:pt idx="56">
-                        <c:v>143605446</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="57">
-                        <c:v>144676368</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="58">
-                        <c:v>161841702</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="59">
-                        <c:v>170508605</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="60">
-                        <c:v>174842161</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="61">
-                        <c:v>177033678</c:v>
+                        <c:v>-8.2304357398441507E-6</c:v>
                       </c:pt>
                       <c:pt idx="62">
-                        <c:v>178099828</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>178636319</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>179176325</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>180245640</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>180787041</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>181846581</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>200870363</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>211532777</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>215825156</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>215834935</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>216913206</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>217453257</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>217723462</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>217848331</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>217926543</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>217965644</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>217985200</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>218019316</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>218084372</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>218213552</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>218500769</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>219124221</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>220193533</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>237354053</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>237359060</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>241587749</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>243729247</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>244784993</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>245315354</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>245585542</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>245720635</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>245785680</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>245820711</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>245840719</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>245875743</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>245940788</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>246075882</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>246341065</c:v>
-                      </c:pt>
-                      <c:pt idx="100">
-                        <c:v>246871433</c:v>
-                      </c:pt>
-                      <c:pt idx="101">
-                        <c:v>247932168</c:v>
+                        <c:v>-5.4869646865811402E-6</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2216,13 +1718,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -2554,832 +2056,710 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1681</v>
+        <v>250100000</v>
       </c>
       <c r="B1">
-        <v>479031</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.5961615353858404E-3</v>
+      </c>
+      <c r="C1">
+        <v>3541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1731</v>
+        <v>450200000</v>
       </c>
       <c r="B2">
-        <v>488804</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-2.9985007496251799E-3</v>
+      </c>
+      <c r="C2">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1881</v>
+        <v>650300000</v>
       </c>
       <c r="B3">
-        <v>508356</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.9990004997501201E-3</v>
+      </c>
+      <c r="C3">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1929</v>
+        <v>850400000</v>
       </c>
       <c r="B4">
-        <v>527908</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2017</v>
+        <v>1450500000</v>
       </c>
       <c r="B5">
-        <v>557236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6.66555574070988E-4</v>
+      </c>
+      <c r="C5">
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2053</v>
+        <v>1650600000</v>
       </c>
       <c r="B6">
-        <v>625669</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.99500249875062E-4</v>
+      </c>
+      <c r="C6">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2053</v>
+        <v>1850700000</v>
       </c>
       <c r="B7">
-        <v>763025</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2053</v>
+        <v>2450800000</v>
       </c>
       <c r="B8">
-        <v>1025455</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.33277787035494E-4</v>
+      </c>
+      <c r="C8">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2052</v>
+        <v>2650900000</v>
       </c>
       <c r="B9">
-        <v>1651136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2050</v>
+        <v>3251000000</v>
       </c>
       <c r="B10">
-        <v>2714582</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.33277787035494E-4</v>
+      </c>
+      <c r="C10">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2030</v>
+        <v>3451100000</v>
       </c>
       <c r="B11">
-        <v>19085976</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2122</v>
+        <v>4051200000</v>
       </c>
       <c r="B12">
-        <v>27316713</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.33277787035494E-4</v>
+      </c>
+      <c r="C12">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1933</v>
+        <v>4251300000</v>
       </c>
       <c r="B13">
-        <v>30947211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2080</v>
+        <v>4851400000</v>
       </c>
       <c r="B14">
-        <v>32763229</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2060</v>
+        <v>6651500000</v>
       </c>
       <c r="B15">
-        <v>33676119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2057</v>
+        <v>12051600000</v>
       </c>
       <c r="B16">
-        <v>34135591</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-3.7036351178681799E-5</v>
+      </c>
+      <c r="C16">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2055</v>
+        <v>12251700000</v>
       </c>
       <c r="B17">
-        <v>34587686</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2051</v>
+        <v>12851800000</v>
       </c>
       <c r="B18">
-        <v>35508332</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2051</v>
+        <v>14651900000</v>
       </c>
       <c r="B19">
-        <v>35958644</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2050</v>
+        <v>20052000000</v>
       </c>
       <c r="B20">
-        <v>36864277</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2030</v>
+        <v>36252100000</v>
       </c>
       <c r="B21">
-        <v>53375782</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-2.4691205609841901E-5</v>
+      </c>
+      <c r="C21">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2122</v>
+        <v>36452200000</v>
       </c>
       <c r="B22">
-        <v>61837068</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1933</v>
+        <v>37052300000</v>
       </c>
       <c r="B23">
-        <v>66061359</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2080</v>
+        <v>38852400000</v>
       </c>
       <c r="B24">
-        <v>68176197</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2060</v>
+        <v>44252500000</v>
       </c>
       <c r="B25">
-        <v>69236980</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2057</v>
+        <v>60452600000</v>
       </c>
       <c r="B26">
-        <v>69764884</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-2.4691205609841901E-5</v>
+      </c>
+      <c r="C26">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2055</v>
+        <v>60652700000</v>
       </c>
       <c r="B27">
-        <v>70296516</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2051</v>
+        <v>61252800000</v>
       </c>
       <c r="B28">
-        <v>71356042</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2051</v>
+        <v>63052900000</v>
       </c>
       <c r="B29">
-        <v>71896041</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2050</v>
+        <v>68453000000</v>
       </c>
       <c r="B30">
-        <v>72956963</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2030</v>
+        <v>84653100000</v>
       </c>
       <c r="B31">
-        <v>89908962</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-2.4691205609841901E-5</v>
+      </c>
+      <c r="C31">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2122</v>
+        <v>84853200000</v>
       </c>
       <c r="B32">
-        <v>98374854</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1933</v>
+        <v>85453300000</v>
       </c>
       <c r="B33">
-        <v>102623009</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2080</v>
+        <v>87253400000</v>
       </c>
       <c r="B34">
-        <v>104767801</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2060</v>
+        <v>92653500000</v>
       </c>
       <c r="B35">
-        <v>105819864</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2057</v>
+        <v>108853600000</v>
       </c>
       <c r="B36">
-        <v>106347438</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-1.23456028049209E-5</v>
+      </c>
+      <c r="C36">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2055</v>
+        <v>109053700000</v>
       </c>
       <c r="B37">
-        <v>106889821</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2051</v>
+        <v>109653800000</v>
       </c>
       <c r="B38">
-        <v>107937140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2051</v>
+        <v>111453900000</v>
       </c>
       <c r="B39">
-        <v>108472270</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2050</v>
+        <v>116854000000</v>
       </c>
       <c r="B40">
-        <v>109533182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2030</v>
+        <v>133054100000</v>
       </c>
       <c r="B41">
-        <v>126575667</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-1.23456028049209E-5</v>
+      </c>
+      <c r="C41">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>2122</v>
+        <v>133254200000</v>
       </c>
       <c r="B42">
-        <v>135088820</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1933</v>
+        <v>133854300000</v>
       </c>
       <c r="B43">
-        <v>139357285</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>2227</v>
+        <v>135654400000</v>
       </c>
       <c r="B44">
-        <v>139357285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>2113</v>
+        <v>141054500000</v>
       </c>
       <c r="B45">
-        <v>140426597</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1733</v>
+        <v>157254600000</v>
       </c>
       <c r="B46">
-        <v>140967058</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-1.23456028049209E-5</v>
+      </c>
+      <c r="C46">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>3533</v>
+        <v>157454700000</v>
       </c>
       <c r="B47">
-        <v>141231009</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>2533</v>
+        <v>158054800000</v>
       </c>
       <c r="B48">
-        <v>141367877</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1621</v>
+        <v>159854900000</v>
       </c>
       <c r="B49">
-        <v>141436310</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2021</v>
+        <v>165255000000</v>
       </c>
       <c r="B50">
-        <v>141475414</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2021</v>
+        <v>181455100000</v>
       </c>
       <c r="B51">
-        <v>141494969</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-1.23456028049209E-5</v>
+      </c>
+      <c r="C51">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2021</v>
+        <v>181655200000</v>
       </c>
       <c r="B52">
-        <v>141524294</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>2057</v>
+        <v>182255300000</v>
       </c>
       <c r="B53">
-        <v>141593663</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>2057</v>
+        <v>184055400000</v>
       </c>
       <c r="B54">
-        <v>141723536</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>2056</v>
+        <v>189455500000</v>
       </c>
       <c r="B55">
-        <v>141987490</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>2054</v>
+        <v>205655600000</v>
       </c>
       <c r="B56">
-        <v>142525174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-1.23456028049209E-5</v>
+      </c>
+      <c r="C56">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>2051</v>
+        <v>205855700000</v>
       </c>
       <c r="B57">
-        <v>143605446</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2050</v>
+        <v>206455800000</v>
       </c>
       <c r="B58">
-        <v>144676368</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>2030</v>
+        <v>208255900000</v>
       </c>
       <c r="B59">
-        <v>161841702</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>2122</v>
+        <v>213656000000</v>
       </c>
       <c r="B60">
-        <v>170508605</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>1933</v>
+        <v>229856100000</v>
       </c>
       <c r="B61">
-        <v>174842161</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2080</v>
+        <v>278456200000</v>
       </c>
       <c r="B62">
-        <v>177033678</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-8.2304357398441507E-6</v>
+      </c>
+      <c r="C62">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>2060</v>
+        <v>424256300000</v>
       </c>
       <c r="B63">
-        <v>178099828</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>2057</v>
-      </c>
-      <c r="B64">
-        <v>178636319</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>2055</v>
-      </c>
-      <c r="B65">
-        <v>179176325</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>2051</v>
-      </c>
-      <c r="B66">
-        <v>180245640</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>2051</v>
-      </c>
-      <c r="B67">
-        <v>180787041</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>2050</v>
-      </c>
-      <c r="B68">
-        <v>181846581</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>2030</v>
-      </c>
-      <c r="B69">
-        <v>200870363</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>2122</v>
-      </c>
-      <c r="B70">
-        <v>211532777</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>1933</v>
-      </c>
-      <c r="B71">
-        <v>215825156</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>2227</v>
-      </c>
-      <c r="B72">
-        <v>215834935</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>2113</v>
-      </c>
-      <c r="B73">
-        <v>216913206</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>1733</v>
-      </c>
-      <c r="B74">
-        <v>217453257</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>3533</v>
-      </c>
-      <c r="B75">
-        <v>217723462</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>2533</v>
-      </c>
-      <c r="B76">
-        <v>217848331</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>1525</v>
-      </c>
-      <c r="B77">
-        <v>217926543</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>2025</v>
-      </c>
-      <c r="B78">
-        <v>217965644</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>2025</v>
-      </c>
-      <c r="B79">
-        <v>217985200</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>2025</v>
-      </c>
-      <c r="B80">
-        <v>218019316</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>2025</v>
-      </c>
-      <c r="B81">
-        <v>218084372</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>2044</v>
-      </c>
-      <c r="B82">
-        <v>218213552</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>2044</v>
-      </c>
-      <c r="B83">
-        <v>218500769</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>2045</v>
-      </c>
-      <c r="B84">
-        <v>219124221</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>2046</v>
-      </c>
-      <c r="B85">
-        <v>220193533</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>2066</v>
-      </c>
-      <c r="B86">
-        <v>237354053</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>1882</v>
-      </c>
-      <c r="B87">
-        <v>237359060</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>2307</v>
-      </c>
-      <c r="B88">
-        <v>241587749</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>1976</v>
-      </c>
-      <c r="B89">
-        <v>243729247</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>2022</v>
-      </c>
-      <c r="B90">
-        <v>244784993</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>2174</v>
-      </c>
-      <c r="B91">
-        <v>245315354</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>1454</v>
-      </c>
-      <c r="B92">
-        <v>245585542</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>3522</v>
-      </c>
-      <c r="B93">
-        <v>245720635</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>690</v>
-      </c>
-      <c r="B94">
-        <v>245785680</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>2040</v>
-      </c>
-      <c r="B95">
-        <v>245820711</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>2040</v>
-      </c>
-      <c r="B96">
-        <v>245840719</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>2040</v>
-      </c>
-      <c r="B97">
-        <v>245875743</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>2040</v>
-      </c>
-      <c r="B98">
-        <v>245940788</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>2040</v>
-      </c>
-      <c r="B99">
-        <v>246075882</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>2041</v>
-      </c>
-      <c r="B100">
-        <v>246341065</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>2043</v>
-      </c>
-      <c r="B101">
-        <v>246871433</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>2046</v>
-      </c>
-      <c r="B102">
-        <v>247932168</v>
+        <v>-5.4869646865811402E-6</v>
+      </c>
+      <c r="C63">
+        <v>2614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>